<commit_message>
Description Step Transformation DATA PBI
</commit_message>
<xml_diff>
--- a/Projet Dekra/Test-data.xlsx
+++ b/Projet Dekra/Test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boudl\Documents\Projet Dekra\PBI_AUTO.github.io\Projet Dekra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503E2B1E-073A-4353-ADA7-B0AE0DD11A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459AACA6-FF84-448C-B77A-67268EA7F80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2F68A4FA-2A69-4B37-9795-E1E7B5594774}"/>
   </bookViews>
@@ -5795,8 +5795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA1D5F2-A3AA-49FA-9963-2019577C3071}">
   <dimension ref="A1:U1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R159" sqref="R159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>